<commit_message>
Add se_trim_sensor.m, Update se_main.m
ADD

se_trim_sensor.m - Trims the Database to  stars within the sensor frame

UPDATE -

se_main.m - add se_trim_sensor.m in mainfile
</commit_message>
<xml_diff>
--- a/Sensor_Modelling/Inputs/se_inputs.xlsx
+++ b/Sensor_Modelling/Inputs/se_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neilabh\Documents\GitHub\STADS_IITBSSP\Sensor_Modelling\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99C521A8-0900-44E0-902E-C0ADD249E59F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CC41908-CF81-4F38-A9F8-C3598AF4BEB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="12960" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -985,7 +985,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>8.9199359999999999</v>
+        <v>24.428527500000001</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -996,7 +996,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>-54.965767999999997</v>
+        <v>-57.236757500000003</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>

</xml_diff>